<commit_message>
db scheme new version
</commit_message>
<xml_diff>
--- a/csv/Notes.xlsx
+++ b/csv/Notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -43,28 +43,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>I loved everything about this museum. The sculpture garden is a great place top sit and relax for a while. The permanent exhibits are spectacular. Although quite crowded, it was never difficult to enjoy the art. Staff are extremely friendly. I'm glad I lived in New York City so that I could visit frequently.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Loved it, I can't wait to come back</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ONCE IN LIFETIME</t>
-  </si>
-  <si>
-    <t>One of those trips(once in a lifetime) you've always dreamed of and we weren't disappointed when had the chance to visit on our honeymoon, with the sun in the sky and a little chilly the views were fab and some great pictures to be taken certainly breathtaking.If your in New York make sure this on your list to visit. Ps the ESB staff were very friendly and helpful well done guys and dolls</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Too modern for me!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The museum is weird. I can't understand most of the works.</t>
+    <t>Loved NY, I can't wait to come back</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -492,95 +477,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.1640625" customWidth="1"/>
-    <col min="4" max="5" width="41.5" customWidth="1"/>
-    <col min="6" max="6" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.33203125" customWidth="1"/>
-    <col min="10" max="10" width="40.1640625" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
-    <col min="12" max="12" width="51.5" customWidth="1"/>
-    <col min="13" max="13" width="60.83203125" customWidth="1"/>
+    <col min="3" max="4" width="41.5" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="40.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="51.5" customWidth="1"/>
+    <col min="11" max="11" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1">
+        <v>20150301</v>
+      </c>
+      <c r="D1">
         <v>0</v>
       </c>
-      <c r="D1" s="1">
-        <v>42064</v>
-      </c>
       <c r="E1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F1">
         <v>1</v>
       </c>
-      <c r="G1">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>42095</v>
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20150502</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>0</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2">
-        <v>42126</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>